<commit_message>
added state maching to shooter excel sheet
</commit_message>
<xml_diff>
--- a/dev/4039.Stronghold.2016.Shooter.xlsx
+++ b/dev/4039.Stronghold.2016.Shooter.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="120" yWindow="120" windowWidth="28140" windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SHOOTER" sheetId="1" r:id="rId1"/>
+    <sheet name="STATE MACHINE" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -278,7 +278,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>SHOOTER!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -306,7 +306,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$481</c:f>
+              <c:f>SHOOTER!$F$2:$F$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -1755,7 +1755,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$481</c:f>
+              <c:f>SHOOTER!$I$2:$I$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -3343,7 +3343,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>SHOOTER!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3357,7 +3357,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$481</c:f>
+              <c:f>SHOOTER!$H$2:$H$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -4806,7 +4806,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$481</c:f>
+              <c:f>SHOOTER!$I$2:$I$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -6387,7 +6387,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>SHOOTER!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6401,7 +6401,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$481</c:f>
+              <c:f>SHOOTER!$F$2:$F$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -7850,7 +7850,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$481</c:f>
+              <c:f>SHOOTER!$H$2:$H$481</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="480"/>
@@ -9498,6 +9498,56 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>35560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>58420</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>35560</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="24" idx="1"/>
+          <a:endCxn id="16" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2247900" y="3591560"/>
+          <a:ext cx="1798320" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -9960,14 +10010,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>71120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -9976,7 +10026,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2260600" y="3060700"/>
+          <a:off x="2260600" y="2984500"/>
           <a:ext cx="1798320" cy="266700"/>
           <a:chOff x="2247900" y="3454400"/>
           <a:chExt cx="1798320" cy="266700"/>
@@ -10035,9 +10085,7 @@
           </a:solidFill>
           <a:ln w="9525" cmpd="sng">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
+              <a:srgbClr val="1F497D"/>
             </a:solidFill>
           </a:ln>
         </xdr:spPr>
@@ -10072,117 +10120,65 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>58420</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="43" name="Group 42"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="2247900" y="3848100"/>
-          <a:ext cx="1798320" cy="266700"/>
-          <a:chOff x="2247900" y="3467100"/>
-          <a:chExt cx="1798320" cy="266700"/>
+          <a:off x="2654300" y="3441700"/>
+          <a:ext cx="1054100" cy="266700"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="39" name="Straight Connector 38"/>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="16" idx="3"/>
-            <a:endCxn id="24" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2247900" y="3591560"/>
-            <a:ext cx="1798320" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="none" w="lg"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="40" name="TextBox 39"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2641600" y="3467100"/>
-            <a:ext cx="1054100" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
           <a:solidFill>
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="tx2"/>
           </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>GP_DOWN</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GP_DOWN</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10478,7 +10474,7 @@
   <dimension ref="A1:M481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -22592,7 +22588,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>